<commit_message>
Changes to be committed: 	deleted:    E3IN_L3_DOC_TYPE_Journal_du_projet_V1.1.docx 	modified:   RISQUES V2.xlsx  Untracked files: 	E3IN_L3_DOC_TYPE_Journal_du_projet_V1.2.docx
</commit_message>
<xml_diff>
--- a/RISQUES V2.xlsx
+++ b/RISQUES V2.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://sccfr-my.sharepoint.com/personal/vdomain_fr_scc_com/Documents/Bureau/Projet L3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdomain\BUGTOUCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="8_{9E9BD836-8CA9-47EA-AEC6-4693B321AFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{18116729-80C9-4FCC-85B2-00122DCD890A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D054C6-28D9-40AC-A000-D76205C4D645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0BD3F82B-97E7-491D-B8BF-A1747B9188EF}"/>
   </bookViews>
@@ -71,9 +71,6 @@
     <t>Détection</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Cyber Attaque</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>Matrice de Risques</t>
+  </si>
+  <si>
+    <t>Indice Criticité</t>
   </si>
 </sst>
 </file>
@@ -331,9 +331,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -361,6 +358,9 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -376,7 +376,7 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -400,6 +400,941 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:radarChart>
+        <c:radarStyle val="marker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Feuil1!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Indice Criticité</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent1">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent1">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Feuil1!$G$4:$G$9</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Maladie</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Limitations du language</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Problème matériel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Manque de materiel</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Transports</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Cyber Attaque</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Feuil1!$L$4:$L$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-256D-45E8-A2F5-A3859F5A7397}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="637965855"/>
+        <c:axId val="637966687"/>
+      </c:radarChart>
+      <c:catAx>
+        <c:axId val="637965855"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="637966687"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="637966687"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="fr-FR"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="637965855"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="accent5">
+          <a:lumMod val="75000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="fr-FR"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="351">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>707668</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>191449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>69273</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Graphique 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EFFFDDA2-36A9-4E88-A2FA-0813B92FA9D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -701,8 +1636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAC4481-A74E-41C4-8DDF-3B99CCCC98C2}">
   <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -757,14 +1692,14 @@
     <row r="2" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="2"/>
       <c r="B2" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2" s="17"/>
       <c r="D2" s="18"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" s="19"/>
       <c r="I2" s="19"/>
@@ -797,30 +1732,30 @@
     </row>
     <row r="3" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="14" t="s">
+      <c r="H3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="J3" s="13" t="s">
         <v>11</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="6" t="s">
-        <v>12</v>
+      <c r="L3" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -848,29 +1783,29 @@
     </row>
     <row r="4" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
-      <c r="B4" s="9" t="s">
-        <v>13</v>
+      <c r="B4" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>3</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="9">
         <v>1</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="9">
         <v>1</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="11">
+      <c r="K4" s="7"/>
+      <c r="L4" s="10">
         <v>3</v>
       </c>
       <c r="M4" s="1"/>
@@ -908,20 +1843,20 @@
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H5" s="7">
+      <c r="G5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" s="6">
         <v>2</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="6">
         <v>2</v>
       </c>
-      <c r="J5" s="7">
+      <c r="J5" s="6">
         <v>2</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="11">
+      <c r="K5" s="7"/>
+      <c r="L5" s="10">
         <v>8</v>
       </c>
       <c r="M5" s="1"/>
@@ -959,20 +1894,20 @@
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="H6" s="10">
+      <c r="G6" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="9">
         <v>5</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="9">
         <v>1</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="9">
         <v>3</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="12">
+      <c r="K6" s="7"/>
+      <c r="L6" s="11">
         <v>15</v>
       </c>
       <c r="M6" s="1"/>
@@ -1005,25 +1940,25 @@
         <v>4</v>
       </c>
       <c r="C7" s="1"/>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="H7" s="7">
+      <c r="G7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6">
         <v>4</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="6">
         <v>2</v>
       </c>
-      <c r="J7" s="7">
+      <c r="J7" s="6">
         <v>2</v>
       </c>
-      <c r="K7" s="8"/>
-      <c r="L7" s="12">
+      <c r="K7" s="7"/>
+      <c r="L7" s="11">
         <v>16</v>
       </c>
       <c r="M7" s="1"/>
@@ -1061,20 +1996,20 @@
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="10">
+      <c r="G8" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="9">
         <v>2</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="9">
         <v>3</v>
       </c>
-      <c r="J8" s="10">
+      <c r="J8" s="9">
         <v>3</v>
       </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="12">
+      <c r="K8" s="7"/>
+      <c r="L8" s="11">
         <v>18</v>
       </c>
       <c r="M8" s="1"/>
@@ -1103,29 +2038,29 @@
     </row>
     <row r="9" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2"/>
-      <c r="B9" s="7" t="s">
-        <v>17</v>
+      <c r="B9" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="21">
+      <c r="G9" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="15">
         <v>3</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="15">
         <v>2</v>
       </c>
-      <c r="J9" s="21">
+      <c r="J9" s="15">
         <v>5</v>
       </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="15">
+      <c r="K9" s="7"/>
+      <c r="L9" s="14">
         <v>30</v>
       </c>
       <c r="M9" s="1"/>
@@ -1229,7 +2164,7 @@
     <row r="12" spans="1:35" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="2"/>
       <c r="B12" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="19"/>
       <c r="D12" s="20"/>
@@ -1267,11 +2202,11 @@
     </row>
     <row r="13" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="2"/>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="12" t="s">
         <v>0</v>
       </c>
       <c r="C13" s="1"/>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="13" t="s">
         <v>1</v>
       </c>
       <c r="E13" s="2"/>
@@ -1308,12 +2243,12 @@
     </row>
     <row r="14" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2"/>
-      <c r="B14" s="9" t="s">
-        <v>13</v>
+      <c r="B14" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1354,7 +2289,7 @@
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -1395,7 +2330,7 @@
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1435,8 +2370,8 @@
         <v>4</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="7" t="s">
-        <v>22</v>
+      <c r="D17" s="6" t="s">
+        <v>21</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -1477,7 +2412,7 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1513,12 +2448,12 @@
     </row>
     <row r="19" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2"/>
-      <c r="B19" s="7" t="s">
-        <v>17</v>
+      <c r="B19" s="6" t="s">
+        <v>16</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2929,5 +3864,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Changes to be committed: 	modified:   RISQUES V2.xlsx  Untracked files: 	"Etat d\342\200\231avancement.pptx" 	metriques sonar.xlsx
</commit_message>
<xml_diff>
--- a/RISQUES V2.xlsx
+++ b/RISQUES V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vdomain\BUGTOUCH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gautier Richaud\BUGTOUCH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03D054C6-28D9-40AC-A000-D76205C4D645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2071666F-7732-4CD8-9A55-082C062AC513}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{0BD3F82B-97E7-491D-B8BF-A1747B9188EF}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{0BD3F82B-97E7-491D-B8BF-A1747B9188EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -86,28 +86,16 @@
     <t>Problème matériel</t>
   </si>
   <si>
-    <t>Actions Curative</t>
-  </si>
-  <si>
-    <t>Actions Préventive</t>
-  </si>
-  <si>
     <t>Partir en avance et prévoir le trafique</t>
   </si>
   <si>
     <t>Se prémunir des maladies via les geste barrières</t>
   </si>
   <si>
-    <t>Sélectionnement d'un langage généraliste</t>
-  </si>
-  <si>
     <t>Commander la matériel manquant</t>
   </si>
   <si>
     <t xml:space="preserve">Prévoir un BackUP du projet et sensibiliser l'équipe à la cyber sécurité </t>
-  </si>
-  <si>
-    <t>Prévois un BackUP et du matériel de rechange si possible</t>
   </si>
   <si>
     <t>Changer ou réparer le matériel défectueux</t>
@@ -120,6 +108,18 @@
   </si>
   <si>
     <t>Indice Criticité</t>
+  </si>
+  <si>
+    <t>Actions Curatives</t>
+  </si>
+  <si>
+    <t>Actions Préventives</t>
+  </si>
+  <si>
+    <t>Sélection d'un langage généraliste</t>
+  </si>
+  <si>
+    <t>Prévoir un BackUP et du matériel de rechange si possible</t>
   </si>
 </sst>
 </file>
@@ -361,6 +361,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -375,9 +378,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -442,7 +442,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="fr-FR"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -637,7 +637,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="637966687"/>
@@ -696,7 +696,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="fr-FR"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="637965855"/>
@@ -743,7 +743,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="fr-FR"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1636,23 +1636,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAC4481-A74E-41C4-8DDF-3B99CCCC98C2}">
   <dimension ref="A1:AI56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="143" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.453125" customWidth="1"/>
-    <col min="3" max="3" width="1.453125" customWidth="1"/>
-    <col min="4" max="4" width="80.453125" customWidth="1"/>
-    <col min="6" max="6" width="10.90625" customWidth="1"/>
-    <col min="7" max="7" width="20.453125" customWidth="1"/>
-    <col min="8" max="10" width="12.6328125" customWidth="1"/>
-    <col min="11" max="11" width="1.26953125" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" customWidth="1"/>
+    <col min="2" max="2" width="39.42578125" customWidth="1"/>
+    <col min="3" max="3" width="1.42578125" customWidth="1"/>
+    <col min="4" max="4" width="80.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" customWidth="1"/>
+    <col min="7" max="7" width="20.42578125" customWidth="1"/>
+    <col min="8" max="10" width="12.5703125" customWidth="1"/>
+    <col min="11" max="11" width="1.28515625" customWidth="1"/>
+    <col min="12" max="12" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:35" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -1689,23 +1689,23 @@
       <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
-      <c r="B2" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="19"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
-      <c r="G2" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="20"/>
+      <c r="G2" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="21"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -1730,7 +1730,7 @@
       <c r="AH2" s="1"/>
       <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="12" t="s">
         <v>0</v>
@@ -1754,8 +1754,8 @@
         <v>11</v>
       </c>
       <c r="K3" s="1"/>
-      <c r="L3" s="21" t="s">
-        <v>28</v>
+      <c r="L3" s="16" t="s">
+        <v>24</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
@@ -1781,14 +1781,14 @@
       <c r="AH3" s="1"/>
       <c r="AI3" s="1"/>
     </row>
-    <row r="4" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="4" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1832,7 +1832,7 @@
       <c r="AH4" s="1"/>
       <c r="AI4" s="1"/>
     </row>
-    <row r="5" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
       <c r="B5" s="3" t="s">
         <v>2</v>
@@ -1883,7 +1883,7 @@
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
     </row>
-    <row r="6" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="5" t="s">
         <v>3</v>
@@ -1934,7 +1934,7 @@
       <c r="AH6" s="1"/>
       <c r="AI6" s="1"/>
     </row>
-    <row r="7" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
       <c r="B7" s="3" t="s">
         <v>4</v>
@@ -1985,7 +1985,7 @@
       <c r="AH7" s="1"/>
       <c r="AI7" s="1"/>
     </row>
-    <row r="8" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="5" t="s">
         <v>5</v>
@@ -2036,14 +2036,14 @@
       <c r="AH8" s="1"/>
       <c r="AI8" s="1"/>
     </row>
-    <row r="9" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -2087,7 +2087,7 @@
       <c r="AH9" s="1"/>
       <c r="AI9" s="1"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2124,7 +2124,7 @@
       <c r="AH10" s="1"/>
       <c r="AI10" s="1"/>
     </row>
-    <row r="11" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -2161,13 +2161,13 @@
       <c r="AH11" s="1"/>
       <c r="AI11" s="1"/>
     </row>
-    <row r="12" spans="1:35" ht="31" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:35" ht="30.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
-      <c r="B12" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
+      <c r="B12" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="1"/>
@@ -2200,7 +2200,7 @@
       <c r="AH12" s="1"/>
       <c r="AI12" s="1"/>
     </row>
-    <row r="13" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:35" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
       <c r="B13" s="12" t="s">
         <v>0</v>
@@ -2241,14 +2241,14 @@
       <c r="AH13" s="1"/>
       <c r="AI13" s="1"/>
     </row>
-    <row r="14" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -2282,14 +2282,14 @@
       <c r="AH14" s="1"/>
       <c r="AI14" s="1"/>
     </row>
-    <row r="15" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -2323,14 +2323,14 @@
       <c r="AH15" s="1"/>
       <c r="AI15" s="1"/>
     </row>
-    <row r="16" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -2364,14 +2364,14 @@
       <c r="AH16" s="1"/>
       <c r="AI16" s="1"/>
     </row>
-    <row r="17" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="6" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -2405,14 +2405,14 @@
       <c r="AH17" s="1"/>
       <c r="AI17" s="1"/>
     </row>
-    <row r="18" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
       <c r="B18" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="5" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -2446,14 +2446,14 @@
       <c r="AH18" s="1"/>
       <c r="AI18" s="1"/>
     </row>
-    <row r="19" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -2487,7 +2487,7 @@
       <c r="AH19" s="1"/>
       <c r="AI19" s="1"/>
     </row>
-    <row r="20" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:35" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -2524,7 +2524,7 @@
       <c r="AH20" s="1"/>
       <c r="AI20" s="1"/>
     </row>
-    <row r="21" spans="1:35" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:35" ht="30.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -2561,7 +2561,7 @@
       <c r="AH21" s="1"/>
       <c r="AI21" s="1"/>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -2598,7 +2598,7 @@
       <c r="AH22" s="1"/>
       <c r="AI22" s="1"/>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2635,7 +2635,7 @@
       <c r="AH23" s="1"/>
       <c r="AI23" s="1"/>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2672,7 +2672,7 @@
       <c r="AH24" s="1"/>
       <c r="AI24" s="1"/>
     </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -2709,7 +2709,7 @@
       <c r="AH25" s="1"/>
       <c r="AI25" s="1"/>
     </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -2746,7 +2746,7 @@
       <c r="AH26" s="1"/>
       <c r="AI26" s="1"/>
     </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -2783,7 +2783,7 @@
       <c r="AH27" s="1"/>
       <c r="AI27" s="1"/>
     </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -2820,7 +2820,7 @@
       <c r="AH28" s="1"/>
       <c r="AI28" s="1"/>
     </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -2857,7 +2857,7 @@
       <c r="AH29" s="1"/>
       <c r="AI29" s="1"/>
     </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -2894,7 +2894,7 @@
       <c r="AH30" s="1"/>
       <c r="AI30" s="1"/>
     </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -2931,7 +2931,7 @@
       <c r="AH31" s="1"/>
       <c r="AI31" s="1"/>
     </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -2968,7 +2968,7 @@
       <c r="AH32" s="1"/>
       <c r="AI32" s="1"/>
     </row>
-    <row r="33" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3005,7 +3005,7 @@
       <c r="AH33" s="1"/>
       <c r="AI33" s="1"/>
     </row>
-    <row r="34" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3042,7 +3042,7 @@
       <c r="AH34" s="1"/>
       <c r="AI34" s="1"/>
     </row>
-    <row r="35" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3079,7 +3079,7 @@
       <c r="AH35" s="1"/>
       <c r="AI35" s="1"/>
     </row>
-    <row r="36" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3116,7 +3116,7 @@
       <c r="AH36" s="1"/>
       <c r="AI36" s="1"/>
     </row>
-    <row r="37" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3153,7 +3153,7 @@
       <c r="AH37" s="1"/>
       <c r="AI37" s="1"/>
     </row>
-    <row r="38" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3190,7 +3190,7 @@
       <c r="AH38" s="1"/>
       <c r="AI38" s="1"/>
     </row>
-    <row r="39" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -3227,7 +3227,7 @@
       <c r="AH39" s="1"/>
       <c r="AI39" s="1"/>
     </row>
-    <row r="40" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3264,7 +3264,7 @@
       <c r="AH40" s="1"/>
       <c r="AI40" s="1"/>
     </row>
-    <row r="41" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3301,7 +3301,7 @@
       <c r="AH41" s="1"/>
       <c r="AI41" s="1"/>
     </row>
-    <row r="42" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3338,7 +3338,7 @@
       <c r="AH42" s="1"/>
       <c r="AI42" s="1"/>
     </row>
-    <row r="43" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3375,7 +3375,7 @@
       <c r="AH43" s="1"/>
       <c r="AI43" s="1"/>
     </row>
-    <row r="44" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3412,7 +3412,7 @@
       <c r="AH44" s="1"/>
       <c r="AI44" s="1"/>
     </row>
-    <row r="45" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3449,7 +3449,7 @@
       <c r="AH45" s="1"/>
       <c r="AI45" s="1"/>
     </row>
-    <row r="46" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -3486,7 +3486,7 @@
       <c r="AH46" s="1"/>
       <c r="AI46" s="1"/>
     </row>
-    <row r="47" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -3523,7 +3523,7 @@
       <c r="AH47" s="1"/>
       <c r="AI47" s="1"/>
     </row>
-    <row r="48" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -3560,7 +3560,7 @@
       <c r="AH48" s="1"/>
       <c r="AI48" s="1"/>
     </row>
-    <row r="49" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -3597,7 +3597,7 @@
       <c r="AH49" s="1"/>
       <c r="AI49" s="1"/>
     </row>
-    <row r="50" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -3634,7 +3634,7 @@
       <c r="AH50" s="1"/>
       <c r="AI50" s="1"/>
     </row>
-    <row r="51" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -3671,7 +3671,7 @@
       <c r="AH51" s="1"/>
       <c r="AI51" s="1"/>
     </row>
-    <row r="52" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -3708,7 +3708,7 @@
       <c r="AH52" s="1"/>
       <c r="AI52" s="1"/>
     </row>
-    <row r="53" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -3745,7 +3745,7 @@
       <c r="AH53" s="1"/>
       <c r="AI53" s="1"/>
     </row>
-    <row r="54" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -3782,7 +3782,7 @@
       <c r="AH54" s="1"/>
       <c r="AI54" s="1"/>
     </row>
-    <row r="55" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -3819,7 +3819,7 @@
       <c r="AH55" s="1"/>
       <c r="AI55" s="1"/>
     </row>
-    <row r="56" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>

</xml_diff>